<commit_message>
Minor change to comment.
</commit_message>
<xml_diff>
--- a/Severn Trent - Operating Model.xlsx
+++ b/Severn Trent - Operating Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\SVT LN Equity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513ECE9A-9FB7-49FF-B27C-1F382942761E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EC7E05-0F8D-46B3-86CF-552D393C9CAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{56836699-8929-4347-9712-56FB534FD4C1}"/>
   </bookViews>
@@ -57,22 +57,6 @@
             <family val="2"/>
           </rPr>
           <t>Inline with guidance</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B117" authorId="0" shapeId="0" xr:uid="{CFC22515-8EEF-40D7-8F3F-AA8CA8FADBF5}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Measured as:
-Base return + Totex Outperformance of Ofwat targets + 
-ODI performance + Financing performance
-All of these performance figures are all relative to targets setforth by Ofwat.</t>
         </r>
       </text>
     </comment>
@@ -3559,14 +3543,14 @@
     <xf numFmtId="0" fontId="24" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -26501,7 +26485,7 @@
   <dimension ref="B2:Q282"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31785,7 +31769,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="eM4uVdTk4b5U4bAePUfDaQo1DfhBdI/OHrZdOsBKX2lvjCEEEbrlKMdj1OS3AnZjLUf4PPSXeh72Y/ZPaRvfQA==" saltValue="hxqBSWmDm0ymaJXjny6beg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="u2fRUFv9J5hW/m6wmDUUJHy2nSPQr7IUb1m9B7WMSuNKYKLIfszStcQJcMGF36sXStBQnkMrBTp6/c1hpobhHw==" saltValue="iWOv4aEq7bYJObDgrJT0Aw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="G74 G147 G185 G204 G168 G37 G145 G201 G15 G262 G11 G143 G139 G162 G164 G166 G21 G19 G50 G52 G172 G175 G177 G199 G196 G43 G253 G255 G257 G259 G26 G28 G30 G13 G17 G182 G180 F57 F98 D57" formula="1"/>
@@ -43876,17 +43860,17 @@
       <c r="H2" s="34"/>
     </row>
     <row r="3" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D3" s="200" t="s">
+      <c r="D3" s="201" t="s">
         <v>413</v>
       </c>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="201"/>
       <c r="H3" s="34"/>
-      <c r="O3" s="200" t="s">
+      <c r="O3" s="201" t="s">
         <v>448</v>
       </c>
-      <c r="P3" s="200"/>
-      <c r="Q3" s="200"/>
+      <c r="P3" s="201"/>
+      <c r="Q3" s="201"/>
       <c r="AA3" s="2" t="s">
         <v>393</v>
       </c>
@@ -43917,11 +43901,11 @@
       <c r="I4" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="K4" s="200" t="s">
+      <c r="K4" s="201" t="s">
         <v>446</v>
       </c>
-      <c r="L4" s="200"/>
-      <c r="M4" s="200"/>
+      <c r="L4" s="201"/>
+      <c r="M4" s="201"/>
       <c r="O4" s="175" t="s">
         <v>450</v>
       </c>
@@ -44137,13 +44121,13 @@
       <c r="AA9" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="AD9" s="201" t="s">
+      <c r="AD9" s="202" t="s">
         <v>825</v>
       </c>
-      <c r="AE9" s="201"/>
-      <c r="AF9" s="201"/>
-      <c r="AG9" s="201"/>
-      <c r="AH9" s="201"/>
+      <c r="AE9" s="202"/>
+      <c r="AF9" s="202"/>
+      <c r="AG9" s="202"/>
+      <c r="AH9" s="202"/>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10" s="108">
@@ -44268,7 +44252,7 @@
       <c r="Q12" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA12" s="202" t="s">
+      <c r="AA12" s="200" t="s">
         <v>393</v>
       </c>
       <c r="AB12" s="191">
@@ -44327,7 +44311,7 @@
       <c r="Q13" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA13" s="202"/>
+      <c r="AA13" s="200"/>
       <c r="AB13" s="191">
         <f>(0.95)*AB14</f>
         <v>874.89899650324253</v>
@@ -44384,7 +44368,7 @@
       <c r="Q14" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA14" s="202" t="s">
+      <c r="AA14" s="200" t="s">
         <v>393</v>
       </c>
       <c r="AB14" s="191">
@@ -44443,7 +44427,7 @@
       <c r="Q15" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA15" s="202"/>
+      <c r="AA15" s="200"/>
       <c r="AB15" s="191">
         <f>1.05*AB14</f>
         <v>966.99362771411018</v>
@@ -44500,7 +44484,7 @@
       <c r="Q16" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA16" s="202"/>
+      <c r="AA16" s="200"/>
       <c r="AB16" s="191">
         <f>1.05*AB15</f>
         <v>1015.3433090998158</v>
@@ -44592,13 +44576,13 @@
       <c r="AA18" s="2" t="s">
         <v>824</v>
       </c>
-      <c r="AD18" s="201" t="s">
+      <c r="AD18" s="202" t="s">
         <v>825</v>
       </c>
-      <c r="AE18" s="201"/>
-      <c r="AF18" s="201"/>
-      <c r="AG18" s="201"/>
-      <c r="AH18" s="201"/>
+      <c r="AE18" s="202"/>
+      <c r="AF18" s="202"/>
+      <c r="AG18" s="202"/>
+      <c r="AH18" s="202"/>
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B19" s="108">
@@ -44715,7 +44699,7 @@
       <c r="Q21" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA21" s="202" t="s">
+      <c r="AA21" s="200" t="s">
         <v>393</v>
       </c>
       <c r="AB21" s="191">
@@ -44774,7 +44758,7 @@
       <c r="Q22" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA22" s="202"/>
+      <c r="AA22" s="200"/>
       <c r="AB22" s="191">
         <f>AB13</f>
         <v>874.89899650324253</v>
@@ -44831,7 +44815,7 @@
       <c r="Q23" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA23" s="202"/>
+      <c r="AA23" s="200"/>
       <c r="AB23" s="191">
         <f>AB14</f>
         <v>920.94631210867635</v>
@@ -44888,7 +44872,7 @@
       <c r="Q24" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA24" s="202"/>
+      <c r="AA24" s="200"/>
       <c r="AB24" s="191">
         <f>AB15</f>
         <v>966.99362771411018</v>
@@ -44945,7 +44929,7 @@
       <c r="Q25" s="178">
         <v>0.11158533728627432</v>
       </c>
-      <c r="AA25" s="202"/>
+      <c r="AA25" s="200"/>
       <c r="AB25" s="191">
         <f>AB16</f>
         <v>1015.3433090998158</v>
@@ -55172,13 +55156,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="joGrTFn7cUt4Bgf5xYj+8+nZI+7njVUjrgpZ+ZxtxQ6L09DESde736W9AsVFHXnbad9YsvPLgDvu2bK3NDXR1w==" saltValue="MrWomFBE0GA49asm4rjH7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
+    <mergeCell ref="AD9:AH9"/>
+    <mergeCell ref="AD18:AH18"/>
     <mergeCell ref="AA21:AA25"/>
     <mergeCell ref="AA12:AA16"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="AD9:AH9"/>
-    <mergeCell ref="AD18:AH18"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>